<commit_message>
[EDIT] correspondance and some fix
</commit_message>
<xml_diff>
--- a/sofraco-back-end/documents/courtier.xlsx
+++ b/sofraco-back-end/documents/courtier.xlsx
@@ -171,7 +171,7 @@
     <t>NEOLIANE</t>
   </si>
   <si>
-    <t>NORTIA (APREP)</t>
+    <t>APREP</t>
   </si>
   <si>
     <t>NOVELIA</t>
@@ -13336,7 +13336,7 @@
       <c r="AU1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AV1" s="3" t="s">
         <v>47</v>
       </c>
       <c r="AW1" s="1" t="s">

</xml_diff>

<commit_message>
[EDIT] fichiers de correspondances
</commit_message>
<xml_diff>
--- a/sofraco-back-end/documents/courtier.xlsx
+++ b/sofraco-back-end/documents/courtier.xlsx
@@ -156,7 +156,7 @@
     <t>SPVIE - AMI TNS</t>
   </si>
   <si>
-    <t>SWISS LIFE</t>
+    <t>SWISSLIFE</t>
   </si>
   <si>
     <t>SWISS LIFE
@@ -60314,7 +60314,9 @@
       </c>
       <c r="AN479" s="10"/>
       <c r="AO479" s="11"/>
-      <c r="AP479" s="10"/>
+      <c r="AP479" s="8">
+        <v>62064.0</v>
+      </c>
       <c r="AQ479" s="8">
         <v>61312.0</v>
       </c>

</xml_diff>